<commit_message>
fix base menu : admin, customer, category, product, supplier, stock
</commit_message>
<xml_diff>
--- a/POSv0/public/template_kategori.xlsx
+++ b/POSv0/public/template_kategori.xlsx
@@ -22,16 +22,16 @@
     <t>kategori_nama</t>
   </si>
   <si>
-    <t>ATK</t>
-  </si>
-  <si>
-    <t>Alat Tulis Kerja</t>
-  </si>
-  <si>
-    <t>CLN</t>
-  </si>
-  <si>
-    <t>Pembersih</t>
+    <t>MPD</t>
+  </si>
+  <si>
+    <t>Makanan Pedas</t>
+  </si>
+  <si>
+    <t>MPM</t>
+  </si>
+  <si>
+    <t>Makanan Pedas Manis</t>
   </si>
 </sst>
 </file>

</xml_diff>